<commit_message>
Adding binary and float16 values
</commit_message>
<xml_diff>
--- a/Data/filters.xlsx
+++ b/Data/filters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borey/Git/HardwareCNN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borey/Git/HardwareCNN/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8638A85-CEB9-9D43-B65B-9E2C8AC5AEF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B081D0-813D-A84E-BA5D-C5C10E2304C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16560" xr2:uid="{FF0C7E42-B71B-004C-BBAB-D3F5F0F9BE04}"/>
+    <workbookView xWindow="240" yWindow="1200" windowWidth="26520" windowHeight="16560" activeTab="1" xr2:uid="{FF0C7E42-B71B-004C-BBAB-D3F5F0F9BE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Filters</t>
   </si>
@@ -59,6 +59,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0000000000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -166,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -175,19 +178,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9ACD49-7910-FC49-B0E8-72602748AADF}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="A1:E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,51 +531,51 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>0.23426208000000001</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="7">
         <v>0.54950743999999996</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="7">
         <v>-0.24479165999999999</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>-0.38058882999999999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7">
+      <c r="A3" s="10"/>
+      <c r="B3" s="5">
         <v>0.60555789999999998</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>-3.4608710000000001E-2</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>0.7735457</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>-0.45489170000000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>3.6434700000000002E-3</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>1.6176010000000001E-2</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <v>1.421032E-2</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>6.9683000000000002E-3</v>
       </c>
     </row>
@@ -584,12 +589,85 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2BCE9D-664D-CA47-803E-D7AF08B3B240}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="5" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11">
+        <v>11001101111111</v>
+      </c>
+      <c r="C2" s="11">
+        <v>11100001100101</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1011001111010100</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1011011000010110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11">
+        <v>11100011011000</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1010100001101110</v>
+      </c>
+      <c r="D3" s="11">
+        <v>11101000110000</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1011011101000110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1101101110110</v>
+      </c>
+      <c r="C4" s="12">
+        <v>10010000100100</v>
+      </c>
+      <c r="D4" s="12">
+        <v>10001101000111</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1111100100011</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>